<commit_message>
updating folder with rebinned scores/data files
</commit_message>
<xml_diff>
--- a/QUAC_USFS/Data_Files/CSV_Files/USFS_QUAC_genalex.xlsx
+++ b/QUAC_USFS/Data_Files/CSV_Files/USFS_QUAC_genalex.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eschumacher\Documents\GitHub\GCC_QUAC_ZAIN\QUAC_USFS\Data_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eschumacher\Documents\GitHub\GCC_QUAC_ZAIN\QUAC_USFS\Data_Files\CSV_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D517CE-6A31-4E54-ABD4-1FE0D04B73D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA372FC6-3A18-4E82-B696-93E4B29CFDE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="246">
   <si>
     <t>DNA_ID</t>
   </si>
@@ -1045,8 +1046,8 @@
   </sheetPr>
   <dimension ref="A1:AF1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1281,10 +1282,10 @@
         <v>232</v>
       </c>
       <c r="W4" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X4" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y4" s="4">
         <v>134</v>
@@ -1379,10 +1380,10 @@
         <v>232</v>
       </c>
       <c r="W5" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X5" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y5" s="4">
         <v>134</v>
@@ -1477,10 +1478,10 @@
         <v>238</v>
       </c>
       <c r="W6" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X6" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y6" s="4">
         <v>134</v>
@@ -1575,10 +1576,10 @@
         <v>232</v>
       </c>
       <c r="W7" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X7" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y7" s="4">
         <v>137</v>
@@ -1673,10 +1674,10 @@
         <v>232</v>
       </c>
       <c r="W8" s="4">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X8" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y8" s="4">
         <v>134</v>
@@ -1771,10 +1772,10 @@
         <v>232</v>
       </c>
       <c r="W9" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X9" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y9" s="4">
         <v>140</v>
@@ -1869,10 +1870,10 @@
         <v>232</v>
       </c>
       <c r="W10" s="4">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X10" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y10" s="4">
         <v>134</v>
@@ -1967,10 +1968,10 @@
         <v>232</v>
       </c>
       <c r="W11" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X11" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y11" s="4">
         <v>134</v>
@@ -2065,10 +2066,10 @@
         <v>232</v>
       </c>
       <c r="W12" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X12" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y12" s="4">
         <v>134</v>
@@ -2163,10 +2164,10 @@
         <v>238</v>
       </c>
       <c r="W13" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X13" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y13" s="3">
         <v>0</v>
@@ -2261,10 +2262,10 @@
         <v>232</v>
       </c>
       <c r="W14" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X14" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y14" s="4">
         <v>134</v>
@@ -2359,10 +2360,10 @@
         <v>232</v>
       </c>
       <c r="W15" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X15" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y15" s="4">
         <v>134</v>
@@ -2457,10 +2458,10 @@
         <v>232</v>
       </c>
       <c r="W16" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X16" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y16" s="4">
         <v>134</v>
@@ -2555,10 +2556,10 @@
         <v>232</v>
       </c>
       <c r="W17" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X17" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y17" s="4">
         <v>137</v>
@@ -2653,10 +2654,10 @@
         <v>232</v>
       </c>
       <c r="W18" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X18" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y18" s="4">
         <v>140</v>
@@ -2751,10 +2752,10 @@
         <v>232</v>
       </c>
       <c r="W19" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X19" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y19" s="4">
         <v>140</v>
@@ -2849,10 +2850,10 @@
         <v>232</v>
       </c>
       <c r="W20" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X20" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y20" s="4">
         <v>140</v>
@@ -2947,10 +2948,10 @@
         <v>232</v>
       </c>
       <c r="W21" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X21" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y21" s="4">
         <v>134</v>
@@ -3045,10 +3046,10 @@
         <v>232</v>
       </c>
       <c r="W22" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X22" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y22" s="4">
         <v>134</v>
@@ -3143,10 +3144,10 @@
         <v>232</v>
       </c>
       <c r="W23" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X23" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y23" s="4">
         <v>134</v>
@@ -3241,10 +3242,10 @@
         <v>238</v>
       </c>
       <c r="W24" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X24" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y24" s="4">
         <v>134</v>
@@ -3339,10 +3340,10 @@
         <v>238</v>
       </c>
       <c r="W25" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X25" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y25" s="4">
         <v>137</v>
@@ -3437,10 +3438,10 @@
         <v>232</v>
       </c>
       <c r="W26" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X26" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y26" s="4">
         <v>137</v>
@@ -3535,10 +3536,10 @@
         <v>232</v>
       </c>
       <c r="W27" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X27" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y27" s="4">
         <v>134</v>
@@ -3633,10 +3634,10 @@
         <v>232</v>
       </c>
       <c r="W28" s="4">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X28" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y28" s="4">
         <v>134</v>
@@ -3731,10 +3732,10 @@
         <v>232</v>
       </c>
       <c r="W29" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X29" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y29" s="4">
         <v>134</v>
@@ -3829,10 +3830,10 @@
         <v>232</v>
       </c>
       <c r="W30" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X30" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y30" s="4">
         <v>134</v>
@@ -3927,10 +3928,10 @@
         <v>232</v>
       </c>
       <c r="W31" s="4">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X31" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y31" s="4">
         <v>134</v>
@@ -4025,10 +4026,10 @@
         <v>232</v>
       </c>
       <c r="W32" s="4">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X32" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y32" s="4">
         <v>137</v>
@@ -4123,10 +4124,10 @@
         <v>232</v>
       </c>
       <c r="W33" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X33" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y33" s="4">
         <v>137</v>
@@ -4221,10 +4222,10 @@
         <v>232</v>
       </c>
       <c r="W34" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X34" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y34" s="4">
         <v>137</v>
@@ -4319,10 +4320,10 @@
         <v>232</v>
       </c>
       <c r="W35" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X35" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y35" s="4">
         <v>137</v>
@@ -4417,10 +4418,10 @@
         <v>232</v>
       </c>
       <c r="W36" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X36" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y36" s="4">
         <v>137</v>
@@ -4515,10 +4516,10 @@
         <v>232</v>
       </c>
       <c r="W37" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X37" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y37" s="4">
         <v>134</v>
@@ -4613,10 +4614,10 @@
         <v>238</v>
       </c>
       <c r="W38" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X38" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y38" s="4">
         <v>137</v>
@@ -4711,10 +4712,10 @@
         <v>232</v>
       </c>
       <c r="W39" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X39" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y39" s="4">
         <v>134</v>
@@ -4809,10 +4810,10 @@
         <v>232</v>
       </c>
       <c r="W40" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X40" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y40" s="4">
         <v>137</v>
@@ -4907,10 +4908,10 @@
         <v>232</v>
       </c>
       <c r="W41" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X41" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y41" s="4">
         <v>137</v>
@@ -5005,10 +5006,10 @@
         <v>232</v>
       </c>
       <c r="W42" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X42" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y42" s="4">
         <v>137</v>
@@ -5103,10 +5104,10 @@
         <v>232</v>
       </c>
       <c r="W43" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X43" s="4">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y43" s="4">
         <v>137</v>
@@ -5201,10 +5202,10 @@
         <v>232</v>
       </c>
       <c r="W44" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X44" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y44" s="4">
         <v>137</v>
@@ -5299,10 +5300,10 @@
         <v>232</v>
       </c>
       <c r="W45" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X45" s="4">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y45" s="4">
         <v>134</v>
@@ -19313,10 +19314,10 @@
         <v>232</v>
       </c>
       <c r="W188" s="7">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X188" s="7">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Y188" s="7">
         <v>137</v>
@@ -24031,4 +24032,1049 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54D78CF-6F59-4B34-A4C9-9A920699ABC4}">
+  <dimension ref="A2:A207"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C207"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>